<commit_message>
adding monthly data for SEB truth model
</commit_message>
<xml_diff>
--- a/projects/SEB_template.xlsx
+++ b/projects/SEB_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="22044" windowHeight="4524" tabRatio="562"/>
+    <workbookView xWindow="-12" yWindow="-12" windowWidth="22044" windowHeight="4524" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2262,9 +2262,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>../../../lib/calibration_data/electric.json</t>
-  </si>
-  <si>
     <t>Variable Name</t>
   </si>
   <si>
@@ -2334,9 +2331,6 @@
     <t>AddMonthlyJSONUtilityDataGas</t>
   </si>
   <si>
-    <t>../../../lib/calibration_data/gas.json</t>
-  </si>
-  <si>
     <t>Gas Bill</t>
   </si>
   <si>
@@ -2818,6 +2812,12 @@
   </si>
   <si>
     <t>SiteEntranceBuildingMorris</t>
+  </si>
+  <si>
+    <t>../../../lib/calibration_data/electric_truth.json</t>
+  </si>
+  <si>
+    <t>../../../lib/calibration_data/gas_truth.json</t>
   </si>
 </sst>
 </file>
@@ -6487,7 +6487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -6645,7 +6645,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>470</v>
@@ -6656,7 +6656,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="22" t="s">
@@ -7126,8 +7126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z124"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7340,7 +7340,7 @@
         <v>739</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>740</v>
+        <v>924</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7348,7 +7348,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>165</v>
@@ -7358,7 +7358,7 @@
         <v>739</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7366,17 +7366,17 @@
         <v>21</v>
       </c>
       <c r="D7" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>743</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>744</v>
       </c>
       <c r="F7" s="39"/>
       <c r="G7" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7384,17 +7384,17 @@
         <v>21</v>
       </c>
       <c r="D8" s="22" t="s">
+        <v>745</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>746</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>747</v>
       </c>
       <c r="F8" s="39"/>
       <c r="G8" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7402,17 +7402,17 @@
         <v>21</v>
       </c>
       <c r="D9" s="22" t="s">
+        <v>748</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>749</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>750</v>
       </c>
       <c r="F9" s="39"/>
       <c r="G9" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7420,17 +7420,17 @@
         <v>21</v>
       </c>
       <c r="D10" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>752</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>753</v>
       </c>
       <c r="F10" s="39"/>
       <c r="G10" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7438,17 +7438,17 @@
         <v>21</v>
       </c>
       <c r="D11" s="22" t="s">
+        <v>754</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>755</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>756</v>
       </c>
       <c r="F11" s="39"/>
       <c r="G11" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I11" s="40" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7456,17 +7456,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="22" t="s">
+        <v>757</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>758</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>759</v>
       </c>
       <c r="F12" s="39"/>
       <c r="G12" s="22" t="s">
         <v>62</v>
       </c>
       <c r="I12" s="40" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7474,17 +7474,17 @@
         <v>21</v>
       </c>
       <c r="D13" s="22" t="s">
+        <v>760</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>761</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>762</v>
       </c>
       <c r="F13" s="39"/>
       <c r="G13" s="22" t="s">
         <v>62</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="37" customFormat="1" x14ac:dyDescent="0.3">
@@ -7492,7 +7492,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>736</v>
@@ -7521,7 +7521,7 @@
         <v>739</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>764</v>
+        <v>925</v>
       </c>
     </row>
     <row r="16" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7529,7 +7529,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>165</v>
@@ -7539,7 +7539,7 @@
         <v>739</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="17" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7547,17 +7547,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="22" t="s">
+        <v>742</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>743</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>744</v>
       </c>
       <c r="F17" s="39"/>
       <c r="G17" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7565,17 +7565,17 @@
         <v>21</v>
       </c>
       <c r="D18" s="22" t="s">
+        <v>745</v>
+      </c>
+      <c r="E18" s="22" t="s">
         <v>746</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>747</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="19" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7583,17 +7583,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="22" t="s">
+        <v>748</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>749</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>750</v>
       </c>
       <c r="F19" s="39"/>
       <c r="G19" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="20" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7601,17 +7601,17 @@
         <v>21</v>
       </c>
       <c r="D20" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="E20" s="22" t="s">
         <v>752</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>753</v>
       </c>
       <c r="F20" s="39"/>
       <c r="G20" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="21" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7619,17 +7619,17 @@
         <v>21</v>
       </c>
       <c r="D21" s="22" t="s">
+        <v>754</v>
+      </c>
+      <c r="E21" s="22" t="s">
         <v>755</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>756</v>
       </c>
       <c r="F21" s="39"/>
       <c r="G21" s="22" t="s">
         <v>739</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="22" spans="1:18" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -7637,17 +7637,17 @@
         <v>21</v>
       </c>
       <c r="D22" s="22" t="s">
+        <v>757</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>758</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>759</v>
       </c>
       <c r="F22" s="39"/>
       <c r="G22" s="22" t="s">
         <v>62</v>
       </c>
       <c r="I22" s="40" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="23" spans="1:18" s="37" customFormat="1" x14ac:dyDescent="0.3">
@@ -7655,13 +7655,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>232</v>
@@ -7713,7 +7713,7 @@
         <v>22</v>
       </c>
       <c r="D26" s="42" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="E26" s="26" t="s">
         <v>69</v>
@@ -7750,10 +7750,10 @@
         <v>21</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="F27" s="39"/>
       <c r="G27" s="21" t="s">
@@ -7768,10 +7768,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="46" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="E28" s="45" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="F28" s="39"/>
       <c r="G28" s="45" t="s">
@@ -7805,10 +7805,10 @@
         <v>21</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="21" t="s">
@@ -7823,10 +7823,10 @@
         <v>21</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F30" s="48"/>
       <c r="G30" s="21" t="s">
@@ -7841,13 +7841,13 @@
         <v>1</v>
       </c>
       <c r="B31" s="55" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C31" s="55" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D31" s="55" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="E31" s="55" t="s">
         <v>67</v>
@@ -7888,10 +7888,10 @@
         <v>22</v>
       </c>
       <c r="D33" s="59" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="E33" s="59" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="F33" s="60"/>
       <c r="G33" s="59" t="s">
@@ -7925,13 +7925,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="55" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="C34" s="55" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D34" s="55" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="E34" s="55" t="s">
         <v>67</v>
@@ -7963,17 +7963,17 @@
         <v>22</v>
       </c>
       <c r="D36" s="65" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="E36" s="65" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="F36" s="60"/>
       <c r="G36" s="65" t="s">
         <v>63</v>
       </c>
       <c r="H36" s="65" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I36" s="61">
         <v>0</v>
@@ -8002,13 +8002,13 @@
         <v>1</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="E37" s="49" t="s">
         <v>67</v>
@@ -8040,17 +8040,17 @@
         <v>22</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F39" s="43"/>
       <c r="G39" s="26" t="s">
         <v>63</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I39" s="26">
         <v>0.8</v>
@@ -8081,13 +8081,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="49" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E40" s="49" t="s">
         <v>67</v>
@@ -8098,7 +8098,7 @@
         <v>21</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="E41" s="21" t="s">
         <v>125</v>
@@ -8119,17 +8119,17 @@
         <v>22</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="F42" s="43"/>
       <c r="G42" s="26" t="s">
         <v>63</v>
       </c>
       <c r="H42" s="26" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I42" s="26">
         <v>4</v>
@@ -8198,7 +8198,7 @@
         <v>22</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="E45" s="26" t="s">
         <v>244</v>
@@ -8208,7 +8208,7 @@
         <v>63</v>
       </c>
       <c r="H45" s="26" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I45" s="26">
         <v>0</v>
@@ -8239,17 +8239,17 @@
         <v>22</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="26" t="s">
         <v>63</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I46" s="26">
         <v>0</v>
@@ -8283,10 +8283,10 @@
         <v>186</v>
       </c>
       <c r="C47" s="49" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="E47" s="49" t="s">
         <v>67</v>
@@ -8297,7 +8297,7 @@
         <v>22</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E48" s="26" t="s">
         <v>189</v>
@@ -8307,7 +8307,7 @@
         <v>63</v>
       </c>
       <c r="H48" s="26" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="I48" s="26">
         <v>0</v>
@@ -8338,7 +8338,7 @@
         <v>22</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="E49" s="26" t="s">
         <v>191</v>
@@ -8348,7 +8348,7 @@
         <v>63</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="I49" s="26">
         <v>0</v>
@@ -8379,7 +8379,7 @@
         <v>21</v>
       </c>
       <c r="D50" s="22" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="E50" s="22" t="s">
         <v>193</v>
@@ -8403,13 +8403,13 @@
         <v>0</v>
       </c>
       <c r="B51" s="52" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D51" s="52" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="E51" s="49" t="s">
         <v>67</v>
@@ -8434,10 +8434,10 @@
       </c>
       <c r="C52" s="48"/>
       <c r="D52" s="48" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="E52" s="48" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F52" s="48"/>
       <c r="G52" s="48" t="s">
@@ -8475,10 +8475,10 @@
       </c>
       <c r="C53" s="48"/>
       <c r="D53" s="48" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E53" s="48" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F53" s="48"/>
       <c r="G53" s="48" t="s">
@@ -8515,10 +8515,10 @@
       </c>
       <c r="C54" s="48"/>
       <c r="D54" s="48" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="E54" s="48" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F54" s="48"/>
       <c r="G54" s="48" t="s">
@@ -8555,13 +8555,13 @@
         <v>1</v>
       </c>
       <c r="B55" s="68" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C55" s="68" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D55" s="68" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E55" s="68" t="s">
         <v>67</v>
@@ -8593,7 +8593,7 @@
         <v>21</v>
       </c>
       <c r="D56" s="71" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="E56" s="71" t="s">
         <v>88</v>
@@ -8602,7 +8602,7 @@
         <v>103</v>
       </c>
       <c r="I56" s="71" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="57" spans="1:26" s="59" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -8610,10 +8610,10 @@
         <v>22</v>
       </c>
       <c r="D57" s="59" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="E57" s="59" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="G57" s="59" t="s">
         <v>63</v>
@@ -8643,13 +8643,13 @@
         <v>0</v>
       </c>
       <c r="B58" s="52" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="C58" s="52" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D58" s="52" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E58" s="49" t="s">
         <v>67</v>
@@ -8674,10 +8674,10 @@
       </c>
       <c r="C59" s="48"/>
       <c r="D59" s="48" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="E59" s="48" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="F59" s="48"/>
       <c r="G59" s="48" t="s">
@@ -8715,10 +8715,10 @@
       </c>
       <c r="C60" s="48"/>
       <c r="D60" s="48" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E60" s="48" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F60" s="48"/>
       <c r="G60" s="48" t="s">
@@ -8755,10 +8755,10 @@
       </c>
       <c r="C61" s="48"/>
       <c r="D61" s="48" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E61" s="48" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F61" s="48"/>
       <c r="G61" s="48" t="s">
@@ -8795,13 +8795,13 @@
         <v>1</v>
       </c>
       <c r="B62" s="68" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C62" s="68" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D62" s="68" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="E62" s="68" t="s">
         <v>67</v>
@@ -8833,7 +8833,7 @@
         <v>21</v>
       </c>
       <c r="D63" s="71" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="E63" s="71" t="s">
         <v>88</v>
@@ -8842,7 +8842,7 @@
         <v>103</v>
       </c>
       <c r="I63" s="71" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="64" spans="1:26" s="59" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -8850,10 +8850,10 @@
         <v>22</v>
       </c>
       <c r="D64" s="59" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E64" s="59" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="G64" s="59" t="s">
         <v>63</v>
@@ -8883,13 +8883,13 @@
         <v>1</v>
       </c>
       <c r="B65" s="49" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="C65" s="49" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D65" s="49" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E65" s="49" t="s">
         <v>67</v>
@@ -8900,17 +8900,17 @@
         <v>21</v>
       </c>
       <c r="D66" s="45" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E66" s="45" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F66" s="39"/>
       <c r="G66" s="45" t="s">
         <v>63</v>
       </c>
       <c r="H66" s="45" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I66" s="45">
         <v>1</v>
@@ -8941,17 +8941,17 @@
         <v>22</v>
       </c>
       <c r="D67" s="26" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="E67" s="26" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="F67" s="43"/>
       <c r="G67" s="26" t="s">
         <v>63</v>
       </c>
       <c r="H67" s="26" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="I67" s="26">
         <v>1450</v>
@@ -8982,13 +8982,13 @@
         <v>0</v>
       </c>
       <c r="B68" s="37" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D68" s="37" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="E68" s="37" t="s">
         <v>232</v>
@@ -9012,7 +9012,7 @@
         <v>1</v>
       </c>
       <c r="B69" s="55" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="C69" s="55" t="s">
         <v>163</v>
@@ -9040,7 +9040,7 @@
         <v>103</v>
       </c>
       <c r="I70" s="57" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="J70" s="74"/>
     </row>
@@ -9058,7 +9058,7 @@
         <v>61</v>
       </c>
       <c r="I71" s="74" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J71" s="74"/>
     </row>
@@ -9067,16 +9067,16 @@
         <v>21</v>
       </c>
       <c r="D72" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E72" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G72" s="39" t="s">
         <v>103</v>
       </c>
       <c r="I72" s="75" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J72" s="74"/>
     </row>
@@ -9085,7 +9085,7 @@
         <v>1</v>
       </c>
       <c r="B73" s="55" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="C73" s="55" t="s">
         <v>163</v>
@@ -9113,7 +9113,7 @@
         <v>103</v>
       </c>
       <c r="I74" s="76" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="J74" s="74"/>
     </row>
@@ -9131,7 +9131,7 @@
         <v>61</v>
       </c>
       <c r="I75" s="74" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J75" s="74"/>
     </row>
@@ -9140,16 +9140,16 @@
         <v>21</v>
       </c>
       <c r="D76" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E76" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G76" s="39" t="s">
         <v>103</v>
       </c>
       <c r="I76" s="57" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J76" s="74"/>
     </row>
@@ -9158,7 +9158,7 @@
         <v>1</v>
       </c>
       <c r="B77" s="55" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C77" s="55" t="s">
         <v>163</v>
@@ -9186,7 +9186,7 @@
         <v>103</v>
       </c>
       <c r="I78" s="75" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="J78" s="74"/>
     </row>
@@ -9204,7 +9204,7 @@
         <v>61</v>
       </c>
       <c r="I79" s="74" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J79" s="74"/>
     </row>
@@ -9213,16 +9213,16 @@
         <v>21</v>
       </c>
       <c r="D80" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E80" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G80" s="39" t="s">
         <v>103</v>
       </c>
       <c r="I80" s="57" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J80" s="74"/>
     </row>
@@ -9231,7 +9231,7 @@
         <v>1</v>
       </c>
       <c r="B81" s="55" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C81" s="55" t="s">
         <v>163</v>
@@ -9259,7 +9259,7 @@
         <v>103</v>
       </c>
       <c r="I82" s="75" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J82" s="74"/>
     </row>
@@ -9277,7 +9277,7 @@
         <v>61</v>
       </c>
       <c r="I83" s="74" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J83" s="74"/>
     </row>
@@ -9286,16 +9286,16 @@
         <v>21</v>
       </c>
       <c r="D84" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E84" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G84" s="39" t="s">
         <v>103</v>
       </c>
       <c r="I84" s="57" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J84" s="74"/>
     </row>
@@ -9304,7 +9304,7 @@
         <v>1</v>
       </c>
       <c r="B85" s="55" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C85" s="55" t="s">
         <v>163</v>
@@ -9332,7 +9332,7 @@
         <v>103</v>
       </c>
       <c r="I86" s="75" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="J86" s="74"/>
     </row>
@@ -9350,7 +9350,7 @@
         <v>61</v>
       </c>
       <c r="I87" s="74" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J87" s="74"/>
     </row>
@@ -9359,16 +9359,16 @@
         <v>21</v>
       </c>
       <c r="D88" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E88" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G88" s="39" t="s">
         <v>103</v>
       </c>
       <c r="I88" s="57" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J88" s="74"/>
     </row>
@@ -9377,7 +9377,7 @@
         <v>1</v>
       </c>
       <c r="B89" s="55" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C89" s="55" t="s">
         <v>163</v>
@@ -9405,7 +9405,7 @@
         <v>103</v>
       </c>
       <c r="I90" s="75" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="J90" s="74"/>
     </row>
@@ -9423,7 +9423,7 @@
         <v>61</v>
       </c>
       <c r="I91" s="74" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="J91" s="74"/>
     </row>
@@ -9432,16 +9432,16 @@
         <v>21</v>
       </c>
       <c r="D92" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E92" s="57" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G92" s="39" t="s">
         <v>103</v>
       </c>
       <c r="I92" s="57" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J92" s="74"/>
     </row>
@@ -9450,13 +9450,13 @@
         <v>1</v>
       </c>
       <c r="B93" s="55" t="s">
+        <v>879</v>
+      </c>
+      <c r="C93" s="55" t="s">
+        <v>880</v>
+      </c>
+      <c r="D93" s="55" t="s">
         <v>881</v>
-      </c>
-      <c r="C93" s="55" t="s">
-        <v>882</v>
-      </c>
-      <c r="D93" s="55" t="s">
-        <v>883</v>
       </c>
       <c r="E93" s="55" t="s">
         <v>232</v>
@@ -9467,16 +9467,16 @@
         <v>21</v>
       </c>
       <c r="D94" s="54" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E94" s="54" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="G94" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I94" s="54" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="95" spans="1:10" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9484,16 +9484,16 @@
         <v>21</v>
       </c>
       <c r="D95" s="57" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E95" s="57" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="G95" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I95" s="57" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="96" spans="1:10" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9501,16 +9501,16 @@
         <v>21</v>
       </c>
       <c r="D96" s="57" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E96" s="57" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="G96" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I96" s="54" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="97" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9518,10 +9518,10 @@
         <v>21</v>
       </c>
       <c r="D97" s="57" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E97" s="57" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="G97" s="54" t="s">
         <v>62</v>
@@ -9535,10 +9535,10 @@
         <v>21</v>
       </c>
       <c r="D98" s="57" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E98" s="57" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="G98" s="54" t="s">
         <v>62</v>
@@ -9552,16 +9552,16 @@
         <v>21</v>
       </c>
       <c r="D99" s="57" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E99" s="57" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="G99" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I99" s="57" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="100" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9569,16 +9569,16 @@
         <v>21</v>
       </c>
       <c r="D100" s="57" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E100" s="57" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="G100" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I100" s="75" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9586,16 +9586,16 @@
         <v>21</v>
       </c>
       <c r="D101" s="57" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E101" s="57" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="G101" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I101" s="57" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9603,16 +9603,16 @@
         <v>21</v>
       </c>
       <c r="D102" s="57" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E102" s="57" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="G102" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I102" s="57" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="103" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9620,10 +9620,10 @@
         <v>21</v>
       </c>
       <c r="D103" s="57" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E103" s="57" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="G103" s="54" t="s">
         <v>63</v>
@@ -9637,10 +9637,10 @@
         <v>21</v>
       </c>
       <c r="D104" s="57" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E104" s="57" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="G104" s="54" t="s">
         <v>63</v>
@@ -9654,10 +9654,10 @@
         <v>21</v>
       </c>
       <c r="D105" s="57" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E105" s="57" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="G105" s="54" t="s">
         <v>62</v>
@@ -9671,10 +9671,10 @@
         <v>21</v>
       </c>
       <c r="D106" s="57" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E106" s="57" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="G106" s="54" t="s">
         <v>62</v>
@@ -9688,10 +9688,10 @@
         <v>21</v>
       </c>
       <c r="D107" s="57" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E107" s="57" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="G107" s="54" t="s">
         <v>62</v>
@@ -9705,10 +9705,10 @@
         <v>21</v>
       </c>
       <c r="D108" s="57" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E108" s="57" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="G108" s="54" t="s">
         <v>62</v>
@@ -9722,13 +9722,13 @@
         <v>1</v>
       </c>
       <c r="B109" s="55" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C109" s="55" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D109" s="55" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E109" s="55" t="s">
         <v>232</v>
@@ -9739,16 +9739,16 @@
         <v>21</v>
       </c>
       <c r="D110" s="54" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E110" s="54" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="G110" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I110" s="54" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9756,16 +9756,16 @@
         <v>21</v>
       </c>
       <c r="D111" s="57" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E111" s="57" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="G111" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I111" s="57" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9773,16 +9773,16 @@
         <v>21</v>
       </c>
       <c r="D112" s="57" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E112" s="57" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="G112" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I112" s="54" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="113" spans="2:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9790,10 +9790,10 @@
         <v>21</v>
       </c>
       <c r="D113" s="57" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E113" s="57" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="G113" s="54" t="s">
         <v>62</v>
@@ -9807,10 +9807,10 @@
         <v>21</v>
       </c>
       <c r="D114" s="57" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E114" s="57" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="G114" s="54" t="s">
         <v>62</v>
@@ -9824,16 +9824,16 @@
         <v>21</v>
       </c>
       <c r="D115" s="57" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E115" s="57" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="G115" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I115" s="57" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="116" spans="2:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9841,16 +9841,16 @@
         <v>21</v>
       </c>
       <c r="D116" s="57" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E116" s="57" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="G116" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I116" s="75" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="117" spans="2:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9858,16 +9858,16 @@
         <v>21</v>
       </c>
       <c r="D117" s="57" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E117" s="57" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="G117" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I117" s="57" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="118" spans="2:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9875,16 +9875,16 @@
         <v>21</v>
       </c>
       <c r="D118" s="57" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E118" s="57" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="G118" s="54" t="s">
         <v>103</v>
       </c>
       <c r="I118" s="57" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="119" spans="2:9" s="57" customFormat="1" x14ac:dyDescent="0.3">
@@ -9892,10 +9892,10 @@
         <v>21</v>
       </c>
       <c r="D119" s="57" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E119" s="57" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="G119" s="54" t="s">
         <v>63</v>
@@ -9909,10 +9909,10 @@
         <v>21</v>
       </c>
       <c r="D120" s="57" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E120" s="57" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="G120" s="54" t="s">
         <v>63</v>
@@ -9926,10 +9926,10 @@
         <v>21</v>
       </c>
       <c r="D121" s="57" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E121" s="57" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="G121" s="54" t="s">
         <v>62</v>
@@ -9943,10 +9943,10 @@
         <v>21</v>
       </c>
       <c r="D122" s="57" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E122" s="57" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="G122" s="54" t="s">
         <v>62</v>
@@ -9960,10 +9960,10 @@
         <v>21</v>
       </c>
       <c r="D123" s="57" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E123" s="57" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="G123" s="54" t="s">
         <v>62</v>
@@ -9977,10 +9977,10 @@
         <v>21</v>
       </c>
       <c r="D124" s="57" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E124" s="57" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="G124" s="54" t="s">
         <v>62</v>
@@ -10126,13 +10126,13 @@
     </row>
     <row r="4" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
+        <v>818</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>819</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>820</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>821</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>822</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>467</v>
@@ -10155,13 +10155,13 @@
     </row>
     <row r="5" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
+        <v>821</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>822</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>823</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>824</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>825</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>467</v>
@@ -10656,7 +10656,7 @@
       <c r="B22" s="15"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>651</v>
@@ -10685,7 +10685,7 @@
       <c r="B23" s="15"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>651</v>
@@ -10714,7 +10714,7 @@
       <c r="B24" s="15"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>651</v>
@@ -10743,7 +10743,7 @@
       <c r="B25" s="15"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>655</v>
@@ -10767,15 +10767,15 @@
     </row>
     <row r="26" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F26" s="21" t="s">
         <v>63</v>
@@ -10796,15 +10796,15 @@
     </row>
     <row r="27" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="F27" s="21" t="s">
         <v>63</v>
@@ -10825,15 +10825,15 @@
     </row>
     <row r="28" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F28" s="22" t="s">
         <v>63</v>
@@ -10853,15 +10853,15 @@
     </row>
     <row r="29" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F29" s="22" t="s">
         <v>63</v>
@@ -10881,15 +10881,15 @@
     </row>
     <row r="30" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F30" s="22" t="s">
         <v>63</v>
@@ -10909,15 +10909,15 @@
     </row>
     <row r="31" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F31" s="22" t="s">
         <v>63</v>
@@ -10937,15 +10937,15 @@
     </row>
     <row r="32" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
       <c r="D32" s="21" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F32" s="22" t="s">
         <v>63</v>
@@ -10965,15 +10965,15 @@
     </row>
     <row r="33" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="F33" s="22" t="s">
         <v>63</v>
@@ -10993,12 +10993,12 @@
     </row>
     <row r="34" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="E34" s="21"/>
       <c r="F34" s="22" t="s">
@@ -11016,12 +11016,12 @@
     </row>
     <row r="35" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
       <c r="D35" s="21" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="E35" s="21"/>
       <c r="F35" s="22" t="s">
@@ -11039,12 +11039,12 @@
     </row>
     <row r="36" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
       <c r="D36" s="21" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="E36" s="21"/>
       <c r="F36" s="22" t="s">
@@ -11062,11 +11062,11 @@
     </row>
     <row r="37" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B37" s="21"/>
       <c r="D37" s="21" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="F37" s="22" t="s">
         <v>63</v>
@@ -11083,10 +11083,10 @@
     </row>
     <row r="38" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="26" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="F38" s="26" t="s">
         <v>63</v>
@@ -11104,10 +11104,10 @@
     </row>
     <row r="39" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="F39" s="26" t="s">
         <v>63</v>
@@ -11125,10 +11125,10 @@
     </row>
     <row r="40" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="26" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F40" s="26" t="s">
         <v>63</v>
@@ -11146,10 +11146,10 @@
     </row>
     <row r="41" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="26" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F41" s="26" t="s">
         <v>63</v>

</xml_diff>